<commit_message>
Changed the scraping to put a race number to sort races by the date they take place
</commit_message>
<xml_diff>
--- a/RaceWebScraper/data/OCRSeries.xlsx
+++ b/RaceWebScraper/data/OCRSeries.xlsx
@@ -448,7 +448,7 @@
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Unbroken Torrevieja 2024</t>
+          <t>1   Unbroken Torrevieja 2024</t>
         </is>
       </c>
       <c r="H1" s="1" t="n"/>
@@ -2263,7 +2263,7 @@
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Unbroken Torrevieja 2024</t>
+          <t>1   Unbroken Torrevieja 2024</t>
         </is>
       </c>
       <c r="H1" s="1" t="n"/>
@@ -3046,7 +3046,7 @@
       <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Unbroken Torrevieja 2024</t>
+          <t>1   Unbroken Torrevieja 2024</t>
         </is>
       </c>
       <c r="J1" s="1" t="n"/>
@@ -8065,7 +8065,7 @@
       <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Unbroken Torrevieja 2024</t>
+          <t>1   Unbroken Torrevieja 2024</t>
         </is>
       </c>
       <c r="J1" s="1" t="n"/>

</xml_diff>

<commit_message>
Minor visual tweaks tot he generated excel fils with the results of the leagues
</commit_message>
<xml_diff>
--- a/RaceWebScraper/data/OCRSeries.xlsx
+++ b/RaceWebScraper/data/OCRSeries.xlsx
@@ -32,15 +32,20 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -48,16 +53,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -445,51 +474,51 @@
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="n"/>
+      <c r="F1" s="2" t="n"/>
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>1   Unbroken Torrevieja 2024</t>
         </is>
       </c>
-      <c r="H1" s="1" t="n"/>
+      <c r="H1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Posición</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Puntos</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Carreras</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>Dorsal</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>Club</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>Tiempo</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr">
         <is>
           <t>Puntos</t>
         </is>
@@ -515,7 +544,7 @@
           <t>GARCIA GOMEZ RUBEN</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="5" t="inlineStr">
         <is>
           <t>DESTROYER BY UNBROKEN PROTEAM</t>
         </is>
@@ -525,7 +554,7 @@
           <t>1</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" s="5" t="n">
         <v>100</v>
       </c>
     </row>
@@ -549,7 +578,7 @@
           <t>NACENTA MERINAS PAU</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="5" t="inlineStr">
         <is>
           <t>SPARTAN PROTEAM</t>
         </is>
@@ -559,7 +588,7 @@
           <t>2</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="H4" s="5" t="n">
         <v>92</v>
       </c>
     </row>
@@ -583,7 +612,7 @@
           <t>lopez baños ruben</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="5" t="inlineStr">
         <is>
           <t>TITAN´S BY UNBROKEN PROTEAM</t>
         </is>
@@ -593,7 +622,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="H5" t="n">
+      <c r="H5" s="5" t="n">
         <v>86</v>
       </c>
     </row>
@@ -617,7 +646,7 @@
           <t>PUIG SANCHEZ ADRIÁ</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="5" t="inlineStr">
         <is>
           <t>APUNT TEAM</t>
         </is>
@@ -627,7 +656,7 @@
           <t>4</t>
         </is>
       </c>
-      <c r="H6" t="n">
+      <c r="H6" s="5" t="n">
         <v>82</v>
       </c>
     </row>
@@ -651,7 +680,7 @@
           <t>peso arzadun JOSE MARIA</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="5" t="inlineStr">
         <is>
           <t>SPARTAN PROTEAM</t>
         </is>
@@ -661,7 +690,7 @@
           <t>5</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" s="5" t="n">
         <v>80</v>
       </c>
     </row>
@@ -685,7 +714,7 @@
           <t>ESTEBAN GARCíA EDU</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="5" t="inlineStr">
         <is>
           <t>NATURSPORT_TC</t>
         </is>
@@ -695,7 +724,7 @@
           <t>6</t>
         </is>
       </c>
-      <c r="H8" t="n">
+      <c r="H8" s="5" t="n">
         <v>79</v>
       </c>
     </row>
@@ -719,7 +748,7 @@
           <t>LAQUECHE SARALEGUI PATRICK</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="5" t="inlineStr">
         <is>
           <t>DENONTZAT</t>
         </is>
@@ -729,7 +758,7 @@
           <t>7</t>
         </is>
       </c>
-      <c r="H9" t="n">
+      <c r="H9" s="5" t="n">
         <v>78</v>
       </c>
     </row>
@@ -753,7 +782,7 @@
           <t>BENITO MARTINEZ PABLO</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="5" t="inlineStr">
         <is>
           <t>T-RACE</t>
         </is>
@@ -763,7 +792,7 @@
           <t>8</t>
         </is>
       </c>
-      <c r="H10" t="n">
+      <c r="H10" s="5" t="n">
         <v>77</v>
       </c>
     </row>
@@ -787,7 +816,7 @@
           <t>SEGURA ABELLAN GORKA</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="5" t="inlineStr">
         <is>
           <t>SPALL</t>
         </is>
@@ -797,7 +826,7 @@
           <t>9</t>
         </is>
       </c>
-      <c r="H11" t="n">
+      <c r="H11" s="5" t="n">
         <v>76</v>
       </c>
     </row>
@@ -821,7 +850,7 @@
           <t>LANDART ECHEVERRíA ASIER</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="5" t="inlineStr">
         <is>
           <t>DENONTZAT</t>
         </is>
@@ -831,7 +860,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="H12" t="n">
+      <c r="H12" s="5" t="n">
         <v>75</v>
       </c>
     </row>
@@ -855,7 +884,7 @@
           <t>LABRADOR MERINO DAVID</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" s="5" t="inlineStr">
         <is>
           <t>BRAVE BULLS POWERED BY CLONAPURE</t>
         </is>
@@ -865,7 +894,7 @@
           <t>11</t>
         </is>
       </c>
-      <c r="H13" t="n">
+      <c r="H13" s="5" t="n">
         <v>74</v>
       </c>
     </row>
@@ -889,7 +918,7 @@
           <t>MUGUIRO MARIñELARENA MIKEL</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" s="5" t="inlineStr">
         <is>
           <t>INDEPENDIENTE</t>
         </is>
@@ -899,7 +928,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="H14" t="n">
+      <c r="H14" s="5" t="n">
         <v>73</v>
       </c>
     </row>
@@ -923,7 +952,7 @@
           <t>peso arzadun imanol</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" s="5" t="inlineStr">
         <is>
           <t>unbroken proteam</t>
         </is>
@@ -933,7 +962,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="H15" t="n">
+      <c r="H15" s="5" t="n">
         <v>72</v>
       </c>
     </row>
@@ -957,7 +986,7 @@
           <t>LLUSIA PRINA PABLO</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" s="5" t="inlineStr">
         <is>
           <t>HUMANIMAL</t>
         </is>
@@ -967,7 +996,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="H16" t="n">
+      <c r="H16" s="5" t="n">
         <v>71</v>
       </c>
     </row>
@@ -991,7 +1020,7 @@
           <t>LAKUNTZA MONTERO ARATZ</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" s="5" t="inlineStr">
         <is>
           <t>DENONTZAT</t>
         </is>
@@ -1001,7 +1030,7 @@
           <t>15</t>
         </is>
       </c>
-      <c r="H17" t="n">
+      <c r="H17" s="5" t="n">
         <v>70</v>
       </c>
     </row>
@@ -1025,7 +1054,7 @@
           <t>MENGUAL PEDRO TOMAS</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" s="5" t="inlineStr">
         <is>
           <t>CONTRA EL DIPG</t>
         </is>
@@ -1035,7 +1064,7 @@
           <t>16</t>
         </is>
       </c>
-      <c r="H18" t="n">
+      <c r="H18" s="5" t="n">
         <v>69</v>
       </c>
     </row>
@@ -1059,7 +1088,7 @@
           <t>GURREA ANDER</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" s="5" t="inlineStr">
         <is>
           <t>DENONTZAT</t>
         </is>
@@ -1069,7 +1098,7 @@
           <t>17</t>
         </is>
       </c>
-      <c r="H19" t="n">
+      <c r="H19" s="5" t="n">
         <v>68</v>
       </c>
     </row>
@@ -1093,7 +1122,7 @@
           <t>ARANGO NOREÑA JUAN</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" s="5" t="inlineStr">
         <is>
           <t>BRAVE BULLS POWERED BY CLONAPURE</t>
         </is>
@@ -1103,7 +1132,7 @@
           <t>18</t>
         </is>
       </c>
-      <c r="H20" t="n">
+      <c r="H20" s="5" t="n">
         <v>67</v>
       </c>
     </row>
@@ -1127,7 +1156,7 @@
           <t>CABRERA SANTANA JOSE EHEDEY</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" s="5" t="inlineStr">
         <is>
           <t>ULTÍMATE OCR</t>
         </is>
@@ -1137,7 +1166,7 @@
           <t>19</t>
         </is>
       </c>
-      <c r="H21" t="n">
+      <c r="H21" s="5" t="n">
         <v>66</v>
       </c>
     </row>
@@ -1161,7 +1190,7 @@
           <t>NAVARRO PLAZAS MARTIN</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" s="5" t="inlineStr">
         <is>
           <t>ESCUELA APRIETA Y DISPARA</t>
         </is>
@@ -1171,7 +1200,7 @@
           <t>20</t>
         </is>
       </c>
-      <c r="H22" t="n">
+      <c r="H22" s="5" t="n">
         <v>65</v>
       </c>
     </row>
@@ -1195,7 +1224,7 @@
           <t>QUESADA GARCIA ANTONIO</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F23" s="5" t="inlineStr">
         <is>
           <t>WOLF DEN CREW</t>
         </is>
@@ -1205,7 +1234,7 @@
           <t>21</t>
         </is>
       </c>
-      <c r="H23" t="n">
+      <c r="H23" s="5" t="n">
         <v>64</v>
       </c>
     </row>
@@ -1229,7 +1258,7 @@
           <t>RAMIREZ GARCIA JUANRA</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="F24" s="5" t="inlineStr">
         <is>
           <t>QUALIS</t>
         </is>
@@ -1239,7 +1268,7 @@
           <t>22</t>
         </is>
       </c>
-      <c r="H24" t="n">
+      <c r="H24" s="5" t="n">
         <v>63</v>
       </c>
     </row>
@@ -1263,7 +1292,7 @@
           <t>PAYá HERREROS JAVI</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="F25" s="5" t="inlineStr">
         <is>
           <t>KIKOTRAINING</t>
         </is>
@@ -1273,7 +1302,7 @@
           <t>23</t>
         </is>
       </c>
-      <c r="H25" t="n">
+      <c r="H25" s="5" t="n">
         <v>62</v>
       </c>
     </row>
@@ -1297,7 +1326,7 @@
           <t>DE PABLO HERNANDEZ RICARDO</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="F26" s="5" t="inlineStr">
         <is>
           <t>T-RACE</t>
         </is>
@@ -1307,7 +1336,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="H26" t="n">
+      <c r="H26" s="5" t="n">
         <v>61</v>
       </c>
     </row>
@@ -1331,7 +1360,7 @@
           <t>MARTINEZ LEONAR GERARD</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="F27" s="5" t="inlineStr">
         <is>
           <t>TEAM XXX BLACK MAMBA</t>
         </is>
@@ -1341,7 +1370,7 @@
           <t>25</t>
         </is>
       </c>
-      <c r="H27" t="n">
+      <c r="H27" s="5" t="n">
         <v>60</v>
       </c>
     </row>
@@ -1365,7 +1394,7 @@
           <t>SEVILLA ÁLVARO</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="F28" s="5" t="inlineStr">
         <is>
           <t>OCREX</t>
         </is>
@@ -1375,7 +1404,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="H28" t="n">
+      <c r="H28" s="5" t="n">
         <v>59</v>
       </c>
     </row>
@@ -1399,7 +1428,7 @@
           <t>VALLE GAMBINO GASTóN</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="F29" s="5" t="inlineStr">
         <is>
           <t>THUNDER RACERS</t>
         </is>
@@ -1409,7 +1438,7 @@
           <t>27</t>
         </is>
       </c>
-      <c r="H29" t="n">
+      <c r="H29" s="5" t="n">
         <v>58</v>
       </c>
     </row>
@@ -1433,7 +1462,7 @@
           <t>ARES VILLALOBOS DANIEL</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="F30" s="5" t="inlineStr">
         <is>
           <t>DENONTZAT</t>
         </is>
@@ -1443,7 +1472,7 @@
           <t>28</t>
         </is>
       </c>
-      <c r="H30" t="n">
+      <c r="H30" s="5" t="n">
         <v>57</v>
       </c>
     </row>
@@ -1467,7 +1496,7 @@
           <t>NAVARRO JAVI</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="F31" s="5" t="inlineStr">
         <is>
           <t>QUALIS</t>
         </is>
@@ -1477,7 +1506,7 @@
           <t>29</t>
         </is>
       </c>
-      <c r="H31" t="n">
+      <c r="H31" s="5" t="n">
         <v>56</v>
       </c>
     </row>
@@ -1501,7 +1530,7 @@
           <t>rubio crespo antonio jose</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="F32" s="5" t="inlineStr">
         <is>
           <t>SOW BY UNBROKEN PROTEAM</t>
         </is>
@@ -1511,7 +1540,7 @@
           <t>30</t>
         </is>
       </c>
-      <c r="H32" t="n">
+      <c r="H32" s="5" t="n">
         <v>55</v>
       </c>
     </row>
@@ -1535,7 +1564,7 @@
           <t>SALERNO EDU</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="F33" s="5" t="inlineStr">
         <is>
           <t>OLYMPUS TEAM ANDORRA</t>
         </is>
@@ -1545,7 +1574,7 @@
           <t>31</t>
         </is>
       </c>
-      <c r="H33" t="n">
+      <c r="H33" s="5" t="n">
         <v>54</v>
       </c>
     </row>
@@ -1569,7 +1598,7 @@
           <t>Del Rio Javier</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="F34" s="5" t="inlineStr">
         <is>
           <t>Brave Bulls Powered by Clonapure</t>
         </is>
@@ -1579,7 +1608,7 @@
           <t>32</t>
         </is>
       </c>
-      <c r="H34" t="n">
+      <c r="H34" s="5" t="n">
         <v>53</v>
       </c>
     </row>
@@ -1603,7 +1632,7 @@
           <t>MORENO CORDOBA ANGEL</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="F35" s="5" t="inlineStr">
         <is>
           <t>T-RACE</t>
         </is>
@@ -1613,7 +1642,7 @@
           <t>33</t>
         </is>
       </c>
-      <c r="H35" t="n">
+      <c r="H35" s="5" t="n">
         <v>52</v>
       </c>
     </row>
@@ -1637,7 +1666,7 @@
           <t>SáENZ JUANCRI</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F36" s="5" t="inlineStr">
         <is>
           <t>INFISIO</t>
         </is>
@@ -1647,7 +1676,7 @@
           <t>34</t>
         </is>
       </c>
-      <c r="H36" t="n">
+      <c r="H36" s="5" t="n">
         <v>51</v>
       </c>
     </row>
@@ -1671,7 +1700,7 @@
           <t>MARTINEZ DE ANTOñANA KOLDO</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="F37" s="5" t="inlineStr">
         <is>
           <t>DENONTZAT</t>
         </is>
@@ -1681,7 +1710,7 @@
           <t>35</t>
         </is>
       </c>
-      <c r="H37" t="n">
+      <c r="H37" s="5" t="n">
         <v>50</v>
       </c>
     </row>
@@ -1705,7 +1734,7 @@
           <t>LLORT BARAIBAR LUIS MIGUEL</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="F38" s="5" t="inlineStr">
         <is>
           <t>THUNDER RACERS</t>
         </is>
@@ -1715,7 +1744,7 @@
           <t>36</t>
         </is>
       </c>
-      <c r="H38" t="n">
+      <c r="H38" s="5" t="n">
         <v>49</v>
       </c>
     </row>
@@ -1739,7 +1768,7 @@
           <t>IZETA QUEREJETA EñAUT</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="F39" s="5" t="inlineStr">
         <is>
           <t>DENONTZAT</t>
         </is>
@@ -1749,7 +1778,7 @@
           <t>37</t>
         </is>
       </c>
-      <c r="H39" t="n">
+      <c r="H39" s="5" t="n">
         <v>48</v>
       </c>
     </row>
@@ -1773,7 +1802,7 @@
           <t>PéREZ MERINO JAVIER</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F40" s="5" t="inlineStr">
         <is>
           <t>T-RACE</t>
         </is>
@@ -1783,7 +1812,7 @@
           <t>38</t>
         </is>
       </c>
-      <c r="H40" t="n">
+      <c r="H40" s="5" t="n">
         <v>47</v>
       </c>
     </row>
@@ -1807,7 +1836,7 @@
           <t>ANDRES CLIMENT MARC</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="F41" s="5" t="inlineStr">
         <is>
           <t>SHERPARTANOS</t>
         </is>
@@ -1817,7 +1846,7 @@
           <t>39</t>
         </is>
       </c>
-      <c r="H41" t="n">
+      <c r="H41" s="5" t="n">
         <v>46</v>
       </c>
     </row>
@@ -1841,7 +1870,7 @@
           <t>GANDARILLAS MUÑOZ JAVIER</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="F42" s="5" t="inlineStr">
         <is>
           <t>T-RACE</t>
         </is>
@@ -1851,7 +1880,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="H42" t="n">
+      <c r="H42" s="5" t="n">
         <v>45</v>
       </c>
     </row>
@@ -1875,7 +1904,7 @@
           <t>MARTIN TOMAS JUAN LORENZO</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="F43" s="5" t="inlineStr">
         <is>
           <t>APUNT TEAM</t>
         </is>
@@ -1885,7 +1914,7 @@
           <t>41</t>
         </is>
       </c>
-      <c r="H43" t="n">
+      <c r="H43" s="5" t="n">
         <v>44</v>
       </c>
     </row>
@@ -1909,7 +1938,7 @@
           <t>JUAREZ ZAPATA DANIEL</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="F44" s="5" t="inlineStr">
         <is>
           <t>RACERS LEGION MURCIA</t>
         </is>
@@ -1919,7 +1948,7 @@
           <t>42</t>
         </is>
       </c>
-      <c r="H44" t="n">
+      <c r="H44" s="5" t="n">
         <v>43</v>
       </c>
     </row>
@@ -1943,7 +1972,7 @@
           <t>BARRADO LOPEZ JUAN MIGUEL</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="F45" s="5" t="inlineStr">
         <is>
           <t>CAFETERíA EL RINCóN</t>
         </is>
@@ -1953,7 +1982,7 @@
           <t>43</t>
         </is>
       </c>
-      <c r="H45" t="n">
+      <c r="H45" s="5" t="n">
         <v>42</v>
       </c>
     </row>
@@ -1977,7 +2006,7 @@
           <t>GUERRERO MACIAS VICTOR</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="F46" s="5" t="inlineStr">
         <is>
           <t>INDEPENDIENTE</t>
         </is>
@@ -1987,7 +2016,7 @@
           <t>44</t>
         </is>
       </c>
-      <c r="H46" t="n">
+      <c r="H46" s="5" t="n">
         <v>41</v>
       </c>
     </row>
@@ -2011,12 +2040,12 @@
           <t>GARCIA SERGIO</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
+      <c r="F47" s="5" t="inlineStr">
         <is>
           <t>THUNDER RACERS</t>
         </is>
       </c>
-      <c r="H47" t="n">
+      <c r="H47" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2040,12 +2069,12 @@
           <t>MARTIN CRUZADO ADRIAN</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="F48" s="5" t="inlineStr">
         <is>
           <t>TITAN´S</t>
         </is>
       </c>
-      <c r="H48" t="n">
+      <c r="H48" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2069,12 +2098,12 @@
           <t>Espejo Carmona Jurgen</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="F49" s="5" t="inlineStr">
         <is>
           <t>Olympus Team Andorra</t>
         </is>
       </c>
-      <c r="H49" t="n">
+      <c r="H49" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2098,12 +2127,12 @@
           <t>VILLAR GARRIDO GONZALO</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="F50" s="5" t="inlineStr">
         <is>
           <t>TITAN´S</t>
         </is>
       </c>
-      <c r="H50" t="n">
+      <c r="H50" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2127,12 +2156,12 @@
           <t>ALONSO GILSANZ JULIáN</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
+      <c r="F51" s="5" t="inlineStr">
         <is>
           <t>LIONSOCR</t>
         </is>
       </c>
-      <c r="H51" t="n">
+      <c r="H51" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2156,12 +2185,12 @@
           <t>MUñOZ GONZáLEZ FRANCISCO</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="F52" s="5" t="inlineStr">
         <is>
           <t>CAFETERíA EL RINCóN</t>
         </is>
       </c>
-      <c r="H52" t="n">
+      <c r="H52" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2185,12 +2214,12 @@
           <t>LARA JAVI</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr">
+      <c r="F53" s="5" t="inlineStr">
         <is>
           <t>KXL CENTRO DE ENTRENAMIENTO</t>
         </is>
       </c>
-      <c r="H53" t="n">
+      <c r="H53" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2214,12 +2243,12 @@
           <t>RUIZ EFREN</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr">
+      <c r="F54" s="5" t="inlineStr">
         <is>
           <t>EstudioFit</t>
         </is>
       </c>
-      <c r="H54" t="n">
+      <c r="H54" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2260,51 +2289,51 @@
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="n"/>
+      <c r="F1" s="2" t="n"/>
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>1   Unbroken Torrevieja 2024</t>
         </is>
       </c>
-      <c r="H1" s="1" t="n"/>
+      <c r="H1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Posición</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Puntos</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Carreras</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>Dorsal</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>Club</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>Tiempo</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr">
         <is>
           <t>Puntos</t>
         </is>
@@ -2330,7 +2359,7 @@
           <t>Velasco ruiz Jéssica</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="5" t="inlineStr">
         <is>
           <t>Brave Bulls Powered by Clonapure</t>
         </is>
@@ -2340,7 +2369,7 @@
           <t>1</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" s="5" t="n">
         <v>100</v>
       </c>
     </row>
@@ -2364,7 +2393,7 @@
           <t>IZQUIERDO YESSICA</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="5" t="inlineStr">
         <is>
           <t>T-RACE</t>
         </is>
@@ -2374,7 +2403,7 @@
           <t>2</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="H4" s="5" t="n">
         <v>92</v>
       </c>
     </row>
@@ -2398,7 +2427,7 @@
           <t>CABALLERO OJEDA MARIANGELA</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="5" t="inlineStr">
         <is>
           <t>BRAVE BULLS POWERED BY CLONAPURE</t>
         </is>
@@ -2408,7 +2437,7 @@
           <t>3</t>
         </is>
       </c>
-      <c r="H5" t="n">
+      <c r="H5" s="5" t="n">
         <v>86</v>
       </c>
     </row>
@@ -2432,7 +2461,7 @@
           <t>COMERAS CHUECA CRISTINA</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="5" t="inlineStr">
         <is>
           <t>OCRARAGON</t>
         </is>
@@ -2442,7 +2471,7 @@
           <t>4</t>
         </is>
       </c>
-      <c r="H6" t="n">
+      <c r="H6" s="5" t="n">
         <v>82</v>
       </c>
     </row>
@@ -2466,7 +2495,7 @@
           <t>VAQUERO IGLESIAS FUENCISLA</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="5" t="inlineStr">
         <is>
           <t>OCR ARAGóN</t>
         </is>
@@ -2476,7 +2505,7 @@
           <t>5</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" s="5" t="n">
         <v>80</v>
       </c>
     </row>
@@ -2500,7 +2529,7 @@
           <t>MARINE RIQUE ARIADNA</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="5" t="inlineStr">
         <is>
           <t>PERCUTEAM BY UNBROKEN PROTEAM</t>
         </is>
@@ -2510,7 +2539,7 @@
           <t>6</t>
         </is>
       </c>
-      <c r="H8" t="n">
+      <c r="H8" s="5" t="n">
         <v>79</v>
       </c>
     </row>
@@ -2534,7 +2563,7 @@
           <t>PALACIOS ARAUZO ALBA ELVIRA</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="5" t="inlineStr">
         <is>
           <t>BRAVE BULLS POWERED BY CLONAPUEE</t>
         </is>
@@ -2544,7 +2573,7 @@
           <t>7</t>
         </is>
       </c>
-      <c r="H9" t="n">
+      <c r="H9" s="5" t="n">
         <v>78</v>
       </c>
     </row>
@@ -2568,7 +2597,7 @@
           <t>AZKUNE ANDREA</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="5" t="inlineStr">
         <is>
           <t>unbroken proteam</t>
         </is>
@@ -2578,7 +2607,7 @@
           <t>8</t>
         </is>
       </c>
-      <c r="H10" t="n">
+      <c r="H10" s="5" t="n">
         <v>77</v>
       </c>
     </row>
@@ -2602,7 +2631,7 @@
           <t>TABOADA MORAN LIBANA</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="5" t="inlineStr">
         <is>
           <t>DENONTZAT</t>
         </is>
@@ -2612,7 +2641,7 @@
           <t>9</t>
         </is>
       </c>
-      <c r="H11" t="n">
+      <c r="H11" s="5" t="n">
         <v>76</v>
       </c>
     </row>
@@ -2636,7 +2665,7 @@
           <t>CANDO CASADO RAQUEL</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="5" t="inlineStr">
         <is>
           <t>THUNDER RACERS</t>
         </is>
@@ -2646,7 +2675,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="H12" t="n">
+      <c r="H12" s="5" t="n">
         <v>75</v>
       </c>
     </row>
@@ -2670,7 +2699,7 @@
           <t>Perez Lazarao Luna</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" s="5" t="inlineStr">
         <is>
           <t>LEYENDAS</t>
         </is>
@@ -2680,7 +2709,7 @@
           <t>11</t>
         </is>
       </c>
-      <c r="H13" t="n">
+      <c r="H13" s="5" t="n">
         <v>74</v>
       </c>
     </row>
@@ -2704,7 +2733,7 @@
           <t>Garcia Escribano Elena</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" s="5" t="inlineStr">
         <is>
           <t>T-CENTER</t>
         </is>
@@ -2714,7 +2743,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="H14" t="n">
+      <c r="H14" s="5" t="n">
         <v>73</v>
       </c>
     </row>
@@ -2738,7 +2767,7 @@
           <t>GARCIA RIBERA MONTSE</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" s="5" t="inlineStr">
         <is>
           <t>THUNDER RACERS</t>
         </is>
@@ -2748,7 +2777,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="H15" t="n">
+      <c r="H15" s="5" t="n">
         <v>72</v>
       </c>
     </row>
@@ -2772,7 +2801,7 @@
           <t>FERNANDEZ HERNANDEZ ALICIA</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" s="5" t="inlineStr">
         <is>
           <t>GLADIATORS</t>
         </is>
@@ -2782,7 +2811,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="H16" t="n">
+      <c r="H16" s="5" t="n">
         <v>71</v>
       </c>
     </row>
@@ -2806,7 +2835,7 @@
           <t>PLANA BECERRA CLÀUDIA</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" s="5" t="inlineStr">
         <is>
           <t>INDEPENDIENTE</t>
         </is>
@@ -2816,7 +2845,7 @@
           <t>15</t>
         </is>
       </c>
-      <c r="H17" t="n">
+      <c r="H17" s="5" t="n">
         <v>70</v>
       </c>
     </row>
@@ -2840,7 +2869,7 @@
           <t>CARITJ I COSTA PATRICIA</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" s="5" t="inlineStr">
         <is>
           <t>APUNT TEAM</t>
         </is>
@@ -2850,7 +2879,7 @@
           <t>16</t>
         </is>
       </c>
-      <c r="H18" t="n">
+      <c r="H18" s="5" t="n">
         <v>69</v>
       </c>
     </row>
@@ -2874,7 +2903,7 @@
           <t>MARTINEZ ORQUIN BRENDA</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" s="5" t="inlineStr">
         <is>
           <t>MEDIEVAL OCR TEAM</t>
         </is>
@@ -2884,7 +2913,7 @@
           <t>17</t>
         </is>
       </c>
-      <c r="H19" t="n">
+      <c r="H19" s="5" t="n">
         <v>68</v>
       </c>
     </row>
@@ -2908,12 +2937,12 @@
           <t>GURCHENKOVA NATALIA</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" s="5" t="inlineStr">
         <is>
           <t>QUALITY TRAINING</t>
         </is>
       </c>
-      <c r="H20" t="n">
+      <c r="H20" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2937,12 +2966,12 @@
           <t>millaruelo laderas marta</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" s="5" t="inlineStr">
         <is>
           <t>OCR ARAGON BY UNBROKEN PROTEAM</t>
         </is>
       </c>
-      <c r="H21" t="n">
+      <c r="H21" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2966,12 +2995,12 @@
           <t>RAMIS NEUS</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" s="5" t="inlineStr">
         <is>
           <t>MALLORCA OCR</t>
         </is>
       </c>
-      <c r="H22" t="n">
+      <c r="H22" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2995,12 +3024,12 @@
           <t>WELLS ELLEN</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F23" s="5" t="inlineStr">
         <is>
           <t>INDEPENDIENTE</t>
         </is>
       </c>
-      <c r="H23" t="n">
+      <c r="H23" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3043,61 +3072,61 @@
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
+      <c r="H1" s="2" t="n"/>
       <c r="I1" s="1" t="inlineStr">
         <is>
           <t>1   Unbroken Torrevieja 2024</t>
         </is>
       </c>
-      <c r="J1" s="1" t="n"/>
+      <c r="J1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Posición</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Puntos</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Carreras</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>Dorsal</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>Club</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>Categoría</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr">
         <is>
           <t>Posición</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="I2" s="3" t="inlineStr">
         <is>
           <t>Tiempo</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>Puntos</t>
         </is>
@@ -3128,12 +3157,13 @@
           <t>FOTLIFIT</t>
         </is>
       </c>
+      <c r="H3" s="5" t="n"/>
       <c r="I3" t="inlineStr">
         <is>
           <t>0:48:33.340000</t>
         </is>
       </c>
-      <c r="J3" t="n">
+      <c r="J3" s="5" t="n">
         <v>100</v>
       </c>
     </row>
@@ -3162,12 +3192,13 @@
           <t>Epic Race</t>
         </is>
       </c>
+      <c r="H4" s="5" t="n"/>
       <c r="I4" t="inlineStr">
         <is>
           <t>0:48:56.260000</t>
         </is>
       </c>
-      <c r="J4" t="n">
+      <c r="J4" s="5" t="n">
         <v>99.2</v>
       </c>
     </row>
@@ -3196,12 +3227,13 @@
           <t>FOT-LI FIT</t>
         </is>
       </c>
+      <c r="H5" s="5" t="n"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>0:50:10.250000</t>
         </is>
       </c>
-      <c r="J5" t="n">
+      <c r="J5" s="5" t="n">
         <v>96.8</v>
       </c>
     </row>
@@ -3230,12 +3262,13 @@
           <t>TITAN´S</t>
         </is>
       </c>
+      <c r="H6" s="5" t="n"/>
       <c r="I6" t="inlineStr">
         <is>
           <t>0:50:15</t>
         </is>
       </c>
-      <c r="J6" t="n">
+      <c r="J6" s="5" t="n">
         <v>96.59999999999999</v>
       </c>
     </row>
@@ -3264,12 +3297,13 @@
           <t>THE NEST BOX</t>
         </is>
       </c>
+      <c r="H7" s="5" t="n"/>
       <c r="I7" t="inlineStr">
         <is>
           <t>0:50:18.360000</t>
         </is>
       </c>
-      <c r="J7" t="n">
+      <c r="J7" s="5" t="n">
         <v>96.5</v>
       </c>
     </row>
@@ -3298,12 +3332,13 @@
           <t>OCR ARAGON</t>
         </is>
       </c>
+      <c r="H8" s="5" t="n"/>
       <c r="I8" t="inlineStr">
         <is>
           <t>0:50:22.870000</t>
         </is>
       </c>
-      <c r="J8" t="n">
+      <c r="J8" s="5" t="n">
         <v>96.40000000000001</v>
       </c>
     </row>
@@ -3332,12 +3367,13 @@
           <t>ZUAS SAB</t>
         </is>
       </c>
+      <c r="H9" s="5" t="n"/>
       <c r="I9" t="inlineStr">
         <is>
           <t>0:50:28.510000</t>
         </is>
       </c>
-      <c r="J9" t="n">
+      <c r="J9" s="5" t="n">
         <v>96.2</v>
       </c>
     </row>
@@ -3366,12 +3402,13 @@
           <t>TURIA RACERS OCR</t>
         </is>
       </c>
+      <c r="H10" s="5" t="n"/>
       <c r="I10" t="inlineStr">
         <is>
           <t>0:50:44.060000</t>
         </is>
       </c>
-      <c r="J10" t="n">
+      <c r="J10" s="5" t="n">
         <v>95.7</v>
       </c>
     </row>
@@ -3400,12 +3437,13 @@
           <t>LEYENDAS OCR</t>
         </is>
       </c>
+      <c r="H11" s="5" t="n"/>
       <c r="I11" t="inlineStr">
         <is>
           <t>0:51:00.360000</t>
         </is>
       </c>
-      <c r="J11" t="n">
+      <c r="J11" s="5" t="n">
         <v>95.2</v>
       </c>
     </row>
@@ -3434,12 +3472,13 @@
           <t>SPORTí</t>
         </is>
       </c>
+      <c r="H12" s="5" t="n"/>
       <c r="I12" t="inlineStr">
         <is>
           <t>0:51:08.560000</t>
         </is>
       </c>
-      <c r="J12" t="n">
+      <c r="J12" s="5" t="n">
         <v>94.90000000000001</v>
       </c>
     </row>
@@ -3468,12 +3507,13 @@
           <t>TITAN’S</t>
         </is>
       </c>
+      <c r="H13" s="5" t="n"/>
       <c r="I13" t="inlineStr">
         <is>
           <t>0:51:23.240000</t>
         </is>
       </c>
-      <c r="J13" t="n">
+      <c r="J13" s="5" t="n">
         <v>94.5</v>
       </c>
     </row>
@@ -3502,12 +3542,13 @@
           <t>RS Training</t>
         </is>
       </c>
+      <c r="H14" s="5" t="n"/>
       <c r="I14" t="inlineStr">
         <is>
           <t>0:52:00.350000</t>
         </is>
       </c>
-      <c r="J14" t="n">
+      <c r="J14" s="5" t="n">
         <v>93.40000000000001</v>
       </c>
     </row>
@@ -3536,12 +3577,13 @@
           <t>QUALIS</t>
         </is>
       </c>
+      <c r="H15" s="5" t="n"/>
       <c r="I15" t="inlineStr">
         <is>
           <t>0:52:26.730000</t>
         </is>
       </c>
-      <c r="J15" t="n">
+      <c r="J15" s="5" t="n">
         <v>92.59999999999999</v>
       </c>
     </row>
@@ -3570,12 +3612,13 @@
           <t>THE NEST BOX</t>
         </is>
       </c>
+      <c r="H16" s="5" t="n"/>
       <c r="I16" t="inlineStr">
         <is>
           <t>0:52:28.540000</t>
         </is>
       </c>
-      <c r="J16" t="n">
+      <c r="J16" s="5" t="n">
         <v>92.5</v>
       </c>
     </row>
@@ -3604,12 +3647,13 @@
           <t>Black Panther</t>
         </is>
       </c>
+      <c r="H17" s="5" t="n"/>
       <c r="I17" t="inlineStr">
         <is>
           <t>0:52:51.220000</t>
         </is>
       </c>
-      <c r="J17" t="n">
+      <c r="J17" s="5" t="n">
         <v>91.90000000000001</v>
       </c>
     </row>
@@ -3638,12 +3682,13 @@
           <t>MIKES GYM</t>
         </is>
       </c>
+      <c r="H18" s="5" t="n"/>
       <c r="I18" t="inlineStr">
         <is>
           <t>0:52:59.540000</t>
         </is>
       </c>
-      <c r="J18" t="n">
+      <c r="J18" s="5" t="n">
         <v>91.59999999999999</v>
       </c>
     </row>
@@ -3672,12 +3717,13 @@
           <t>Mallorca OCR</t>
         </is>
       </c>
+      <c r="H19" s="5" t="n"/>
       <c r="I19" t="inlineStr">
         <is>
           <t>0:53:09.540000</t>
         </is>
       </c>
-      <c r="J19" t="n">
+      <c r="J19" s="5" t="n">
         <v>91.3</v>
       </c>
     </row>
@@ -3706,12 +3752,13 @@
           <t>Epic Race</t>
         </is>
       </c>
+      <c r="H20" s="5" t="n"/>
       <c r="I20" t="inlineStr">
         <is>
           <t>0:53:11.550000</t>
         </is>
       </c>
-      <c r="J20" t="n">
+      <c r="J20" s="5" t="n">
         <v>91.3</v>
       </c>
     </row>
@@ -3740,12 +3787,13 @@
           <t>Brave Bulls Powered by Clonapure</t>
         </is>
       </c>
+      <c r="H21" s="5" t="n"/>
       <c r="I21" t="inlineStr">
         <is>
           <t>0:53:17.040000</t>
         </is>
       </c>
-      <c r="J21" t="n">
+      <c r="J21" s="5" t="n">
         <v>91.09999999999999</v>
       </c>
     </row>
@@ -3774,12 +3822,13 @@
           <t>ZUAS SAB</t>
         </is>
       </c>
+      <c r="H22" s="5" t="n"/>
       <c r="I22" t="inlineStr">
         <is>
           <t>0:53:26.970000</t>
         </is>
       </c>
-      <c r="J22" t="n">
+      <c r="J22" s="5" t="n">
         <v>90.8</v>
       </c>
     </row>
@@ -3808,12 +3857,13 @@
           <t>DENONTZAT</t>
         </is>
       </c>
+      <c r="H23" s="5" t="n"/>
       <c r="I23" t="inlineStr">
         <is>
           <t>0:53:28.720000</t>
         </is>
       </c>
-      <c r="J23" t="n">
+      <c r="J23" s="5" t="n">
         <v>90.8</v>
       </c>
     </row>
@@ -3842,12 +3892,13 @@
           <t>Brave Bulls Powered by Clonapure</t>
         </is>
       </c>
+      <c r="H24" s="5" t="n"/>
       <c r="I24" t="inlineStr">
         <is>
           <t>0:53:55.080000</t>
         </is>
       </c>
-      <c r="J24" t="n">
+      <c r="J24" s="5" t="n">
         <v>90.09999999999999</v>
       </c>
     </row>
@@ -3876,12 +3927,13 @@
           <t>RACERS LEGIóN MURCIA</t>
         </is>
       </c>
+      <c r="H25" s="5" t="n"/>
       <c r="I25" t="inlineStr">
         <is>
           <t>0:54:26.960000</t>
         </is>
       </c>
-      <c r="J25" t="n">
+      <c r="J25" s="5" t="n">
         <v>89.2</v>
       </c>
     </row>
@@ -3910,12 +3962,13 @@
           <t>PERCUTEAM</t>
         </is>
       </c>
+      <c r="H26" s="5" t="n"/>
       <c r="I26" t="inlineStr">
         <is>
           <t>0:54:46</t>
         </is>
       </c>
-      <c r="J26" t="n">
+      <c r="J26" s="5" t="n">
         <v>88.7</v>
       </c>
     </row>
@@ -3944,12 +3997,13 @@
           <t>SHERPARTANOS CRONOS GYM</t>
         </is>
       </c>
+      <c r="H27" s="5" t="n"/>
       <c r="I27" t="inlineStr">
         <is>
           <t>0:54:47.550000</t>
         </is>
       </c>
-      <c r="J27" t="n">
+      <c r="J27" s="5" t="n">
         <v>88.59999999999999</v>
       </c>
     </row>
@@ -3978,12 +4032,13 @@
           <t>Mallorca OCR - RS Training</t>
         </is>
       </c>
+      <c r="H28" s="5" t="n"/>
       <c r="I28" t="inlineStr">
         <is>
           <t>0:55:12.960000</t>
         </is>
       </c>
-      <c r="J28" t="n">
+      <c r="J28" s="5" t="n">
         <v>87.90000000000001</v>
       </c>
     </row>
@@ -4012,12 +4067,13 @@
           <t>MALLORCA OCR</t>
         </is>
       </c>
+      <c r="H29" s="5" t="n"/>
       <c r="I29" t="inlineStr">
         <is>
           <t>0:55:14.270000</t>
         </is>
       </c>
-      <c r="J29" t="n">
+      <c r="J29" s="5" t="n">
         <v>87.90000000000001</v>
       </c>
     </row>
@@ -4046,12 +4102,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H30" s="5" t="n"/>
       <c r="I30" t="inlineStr">
         <is>
           <t>0:55:21.380000</t>
         </is>
       </c>
-      <c r="J30" t="n">
+      <c r="J30" s="5" t="n">
         <v>87.7</v>
       </c>
     </row>
@@ -4080,12 +4137,13 @@
           <t>MEDIEVAL OCR TEAM</t>
         </is>
       </c>
+      <c r="H31" s="5" t="n"/>
       <c r="I31" t="inlineStr">
         <is>
           <t>0:55:25.080000</t>
         </is>
       </c>
-      <c r="J31" t="n">
+      <c r="J31" s="5" t="n">
         <v>87.59999999999999</v>
       </c>
     </row>
@@ -4114,12 +4172,13 @@
           <t>Black panter</t>
         </is>
       </c>
+      <c r="H32" s="5" t="n"/>
       <c r="I32" t="inlineStr">
         <is>
           <t>0:55:30.820000</t>
         </is>
       </c>
-      <c r="J32" t="n">
+      <c r="J32" s="5" t="n">
         <v>87.5</v>
       </c>
     </row>
@@ -4148,12 +4207,13 @@
           <t>RACERS LEGION ALICANTE</t>
         </is>
       </c>
+      <c r="H33" s="5" t="n"/>
       <c r="I33" t="inlineStr">
         <is>
           <t>0:55:40.280000</t>
         </is>
       </c>
-      <c r="J33" t="n">
+      <c r="J33" s="5" t="n">
         <v>87.2</v>
       </c>
     </row>
@@ -4182,12 +4242,13 @@
           <t>QUALIS</t>
         </is>
       </c>
+      <c r="H34" s="5" t="n"/>
       <c r="I34" t="inlineStr">
         <is>
           <t>0:55:42.450000</t>
         </is>
       </c>
-      <c r="J34" t="n">
+      <c r="J34" s="5" t="n">
         <v>87.2</v>
       </c>
     </row>
@@ -4216,12 +4277,13 @@
           <t>T-RACE</t>
         </is>
       </c>
+      <c r="H35" s="5" t="n"/>
       <c r="I35" t="inlineStr">
         <is>
           <t>0:55:45.210000</t>
         </is>
       </c>
-      <c r="J35" t="n">
+      <c r="J35" s="5" t="n">
         <v>87.09999999999999</v>
       </c>
     </row>
@@ -4250,12 +4312,13 @@
           <t>OCR ARAGON</t>
         </is>
       </c>
+      <c r="H36" s="5" t="n"/>
       <c r="I36" t="inlineStr">
         <is>
           <t>0:55:59.570000</t>
         </is>
       </c>
-      <c r="J36" t="n">
+      <c r="J36" s="5" t="n">
         <v>86.7</v>
       </c>
     </row>
@@ -4284,12 +4347,13 @@
           <t>RACERS LEGION MURCIA</t>
         </is>
       </c>
+      <c r="H37" s="5" t="n"/>
       <c r="I37" t="inlineStr">
         <is>
           <t>0:56:13.260000</t>
         </is>
       </c>
-      <c r="J37" t="n">
+      <c r="J37" s="5" t="n">
         <v>86.40000000000001</v>
       </c>
     </row>
@@ -4318,12 +4382,13 @@
           <t>MALLORCA OCR</t>
         </is>
       </c>
+      <c r="H38" s="5" t="n"/>
       <c r="I38" t="inlineStr">
         <is>
           <t>0:56:15.270000</t>
         </is>
       </c>
-      <c r="J38" t="n">
+      <c r="J38" s="5" t="n">
         <v>86.3</v>
       </c>
     </row>
@@ -4352,12 +4417,13 @@
           <t>TITAN'S</t>
         </is>
       </c>
+      <c r="H39" s="5" t="n"/>
       <c r="I39" t="inlineStr">
         <is>
           <t>0:56:19.210000</t>
         </is>
       </c>
-      <c r="J39" t="n">
+      <c r="J39" s="5" t="n">
         <v>86.2</v>
       </c>
     </row>
@@ -4386,12 +4452,13 @@
           <t>OCR ARABA</t>
         </is>
       </c>
+      <c r="H40" s="5" t="n"/>
       <c r="I40" t="inlineStr">
         <is>
           <t>0:56:24.250000</t>
         </is>
       </c>
-      <c r="J40" t="n">
+      <c r="J40" s="5" t="n">
         <v>86.09999999999999</v>
       </c>
     </row>
@@ -4420,12 +4487,13 @@
           <t>MIKES GYM</t>
         </is>
       </c>
+      <c r="H41" s="5" t="n"/>
       <c r="I41" t="inlineStr">
         <is>
           <t>0:56:32.560000</t>
         </is>
       </c>
-      <c r="J41" t="n">
+      <c r="J41" s="5" t="n">
         <v>85.90000000000001</v>
       </c>
     </row>
@@ -4454,12 +4522,13 @@
           <t>RACERS LEGIóN MURCIA</t>
         </is>
       </c>
+      <c r="H42" s="5" t="n"/>
       <c r="I42" t="inlineStr">
         <is>
           <t>0:56:33.440000</t>
         </is>
       </c>
-      <c r="J42" t="n">
+      <c r="J42" s="5" t="n">
         <v>85.90000000000001</v>
       </c>
     </row>
@@ -4488,12 +4557,13 @@
           <t>WARRIORS TEAM</t>
         </is>
       </c>
+      <c r="H43" s="5" t="n"/>
       <c r="I43" t="inlineStr">
         <is>
           <t>0:56:36.120000</t>
         </is>
       </c>
-      <c r="J43" t="n">
+      <c r="J43" s="5" t="n">
         <v>85.8</v>
       </c>
     </row>
@@ -4522,12 +4592,13 @@
           <t>PERCUTEAM</t>
         </is>
       </c>
+      <c r="H44" s="5" t="n"/>
       <c r="I44" t="inlineStr">
         <is>
           <t>0:56:36.440000</t>
         </is>
       </c>
-      <c r="J44" t="n">
+      <c r="J44" s="5" t="n">
         <v>85.8</v>
       </c>
     </row>
@@ -4556,12 +4627,13 @@
           <t>TEAM XXX BLACK MAMBA</t>
         </is>
       </c>
+      <c r="H45" s="5" t="n"/>
       <c r="I45" t="inlineStr">
         <is>
           <t>0:56:36.770000</t>
         </is>
       </c>
-      <c r="J45" t="n">
+      <c r="J45" s="5" t="n">
         <v>85.8</v>
       </c>
     </row>
@@ -4590,12 +4662,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H46" s="5" t="n"/>
       <c r="I46" t="inlineStr">
         <is>
           <t>0:56:49.210000</t>
         </is>
       </c>
-      <c r="J46" t="n">
+      <c r="J46" s="5" t="n">
         <v>85.5</v>
       </c>
     </row>
@@ -4624,12 +4697,13 @@
           <t>RACERS LEGION MURCIA</t>
         </is>
       </c>
+      <c r="H47" s="5" t="n"/>
       <c r="I47" t="inlineStr">
         <is>
           <t>0:56:59.560000</t>
         </is>
       </c>
-      <c r="J47" t="n">
+      <c r="J47" s="5" t="n">
         <v>85.2</v>
       </c>
     </row>
@@ -4658,12 +4732,13 @@
           <t>GLADIATORS TEAM</t>
         </is>
       </c>
+      <c r="H48" s="5" t="n"/>
       <c r="I48" t="inlineStr">
         <is>
           <t>0:57:04.160000</t>
         </is>
       </c>
-      <c r="J48" t="n">
+      <c r="J48" s="5" t="n">
         <v>85.09999999999999</v>
       </c>
     </row>
@@ -4692,12 +4767,13 @@
           <t>ATENEA OCR TEAM BY UNBROKEN TEAM</t>
         </is>
       </c>
+      <c r="H49" s="5" t="n"/>
       <c r="I49" t="inlineStr">
         <is>
           <t>0:57:07.250000</t>
         </is>
       </c>
-      <c r="J49" t="n">
+      <c r="J49" s="5" t="n">
         <v>85</v>
       </c>
     </row>
@@ -4726,12 +4802,13 @@
           <t>OCR ARAGON</t>
         </is>
       </c>
+      <c r="H50" s="5" t="n"/>
       <c r="I50" t="inlineStr">
         <is>
           <t>0:57:20.090000</t>
         </is>
       </c>
-      <c r="J50" t="n">
+      <c r="J50" s="5" t="n">
         <v>84.7</v>
       </c>
     </row>
@@ -4760,12 +4837,13 @@
           <t>STRONGFITTESTBOX-OCRTEAM</t>
         </is>
       </c>
+      <c r="H51" s="5" t="n"/>
       <c r="I51" t="inlineStr">
         <is>
           <t>0:57:53.420000</t>
         </is>
       </c>
-      <c r="J51" t="n">
+      <c r="J51" s="5" t="n">
         <v>83.90000000000001</v>
       </c>
     </row>
@@ -4794,12 +4872,13 @@
           <t>BRAVE BULLS BY CLONAPURE</t>
         </is>
       </c>
+      <c r="H52" s="5" t="n"/>
       <c r="I52" t="inlineStr">
         <is>
           <t>0:58:10.490000</t>
         </is>
       </c>
-      <c r="J52" t="n">
+      <c r="J52" s="5" t="n">
         <v>83.5</v>
       </c>
     </row>
@@ -4828,12 +4907,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H53" s="5" t="n"/>
       <c r="I53" t="inlineStr">
         <is>
           <t>0:58:25.160000</t>
         </is>
       </c>
-      <c r="J53" t="n">
+      <c r="J53" s="5" t="n">
         <v>83.09999999999999</v>
       </c>
     </row>
@@ -4862,12 +4942,13 @@
           <t>TURIA RACERS</t>
         </is>
       </c>
+      <c r="H54" s="5" t="n"/>
       <c r="I54" t="inlineStr">
         <is>
           <t>0:58:30.910000</t>
         </is>
       </c>
-      <c r="J54" t="n">
+      <c r="J54" s="5" t="n">
         <v>83</v>
       </c>
     </row>
@@ -4896,12 +4977,13 @@
           <t>Mallorca Ocr</t>
         </is>
       </c>
+      <c r="H55" s="5" t="n"/>
       <c r="I55" t="inlineStr">
         <is>
           <t>0:58:35.500000</t>
         </is>
       </c>
-      <c r="J55" t="n">
+      <c r="J55" s="5" t="n">
         <v>82.90000000000001</v>
       </c>
     </row>
@@ -4930,12 +5012,13 @@
           <t>WOLF DEN CREW</t>
         </is>
       </c>
+      <c r="H56" s="5" t="n"/>
       <c r="I56" t="inlineStr">
         <is>
           <t>0:58:37.930000</t>
         </is>
       </c>
-      <c r="J56" t="n">
+      <c r="J56" s="5" t="n">
         <v>82.8</v>
       </c>
     </row>
@@ -4964,12 +5047,13 @@
           <t>BRAVE BULLS POWERED BY CLONAPUEE</t>
         </is>
       </c>
+      <c r="H57" s="5" t="n"/>
       <c r="I57" t="inlineStr">
         <is>
           <t>0:58:51.410000</t>
         </is>
       </c>
-      <c r="J57" t="n">
+      <c r="J57" s="5" t="n">
         <v>82.5</v>
       </c>
     </row>
@@ -4998,12 +5082,13 @@
           <t>OCR ARAGóN</t>
         </is>
       </c>
+      <c r="H58" s="5" t="n"/>
       <c r="I58" t="inlineStr">
         <is>
           <t>0:59:08.980000</t>
         </is>
       </c>
-      <c r="J58" t="n">
+      <c r="J58" s="5" t="n">
         <v>82.09999999999999</v>
       </c>
     </row>
@@ -5032,12 +5117,13 @@
           <t>OCR ARABA</t>
         </is>
       </c>
+      <c r="H59" s="5" t="n"/>
       <c r="I59" t="inlineStr">
         <is>
           <t>0:59:14.750000</t>
         </is>
       </c>
-      <c r="J59" t="n">
+      <c r="J59" s="5" t="n">
         <v>82</v>
       </c>
     </row>
@@ -5066,12 +5152,13 @@
           <t>FOT-LI FIT</t>
         </is>
       </c>
+      <c r="H60" s="5" t="n"/>
       <c r="I60" t="inlineStr">
         <is>
           <t>0:59:29.910000</t>
         </is>
       </c>
-      <c r="J60" t="n">
+      <c r="J60" s="5" t="n">
         <v>81.59999999999999</v>
       </c>
     </row>
@@ -5100,12 +5187,13 @@
           <t>TKONGS OCR</t>
         </is>
       </c>
+      <c r="H61" s="5" t="n"/>
       <c r="I61" t="inlineStr">
         <is>
           <t>0:59:53.470000</t>
         </is>
       </c>
-      <c r="J61" t="n">
+      <c r="J61" s="5" t="n">
         <v>81.09999999999999</v>
       </c>
     </row>
@@ -5134,12 +5222,13 @@
           <t>Mallorca OCR</t>
         </is>
       </c>
+      <c r="H62" s="5" t="n"/>
       <c r="I62" t="inlineStr">
         <is>
           <t>1:00:10.470000</t>
         </is>
       </c>
-      <c r="J62" t="n">
+      <c r="J62" s="5" t="n">
         <v>80.7</v>
       </c>
     </row>
@@ -5168,12 +5257,13 @@
           <t>DENONTZAT IRUN</t>
         </is>
       </c>
+      <c r="H63" s="5" t="n"/>
       <c r="I63" t="inlineStr">
         <is>
           <t>1:00:32.900000</t>
         </is>
       </c>
-      <c r="J63" t="n">
+      <c r="J63" s="5" t="n">
         <v>80.2</v>
       </c>
     </row>
@@ -5202,12 +5292,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H64" s="5" t="n"/>
       <c r="I64" t="inlineStr">
         <is>
           <t>1:00:47.730000</t>
         </is>
       </c>
-      <c r="J64" t="n">
+      <c r="J64" s="5" t="n">
         <v>79.90000000000001</v>
       </c>
     </row>
@@ -5236,12 +5327,13 @@
           <t>THUNDER RACERS</t>
         </is>
       </c>
+      <c r="H65" s="5" t="n"/>
       <c r="I65" t="inlineStr">
         <is>
           <t>1:01:01.220000</t>
         </is>
       </c>
-      <c r="J65" t="n">
+      <c r="J65" s="5" t="n">
         <v>79.59999999999999</v>
       </c>
     </row>
@@ -5270,12 +5362,13 @@
           <t>DENONTZAT</t>
         </is>
       </c>
+      <c r="H66" s="5" t="n"/>
       <c r="I66" t="inlineStr">
         <is>
           <t>1:01:01.720000</t>
         </is>
       </c>
-      <c r="J66" t="n">
+      <c r="J66" s="5" t="n">
         <v>79.59999999999999</v>
       </c>
     </row>
@@ -5304,12 +5397,13 @@
           <t>MEDIEVAL OCR TEAM</t>
         </is>
       </c>
+      <c r="H67" s="5" t="n"/>
       <c r="I67" t="inlineStr">
         <is>
           <t>1:01:11.640000</t>
         </is>
       </c>
-      <c r="J67" t="n">
+      <c r="J67" s="5" t="n">
         <v>79.3</v>
       </c>
     </row>
@@ -5338,12 +5432,13 @@
           <t>EPIC RACE</t>
         </is>
       </c>
+      <c r="H68" s="5" t="n"/>
       <c r="I68" t="inlineStr">
         <is>
           <t>1:01:18.180000</t>
         </is>
       </c>
-      <c r="J68" t="n">
+      <c r="J68" s="5" t="n">
         <v>79.2</v>
       </c>
     </row>
@@ -5372,12 +5467,13 @@
           <t>OCR ARAGON</t>
         </is>
       </c>
+      <c r="H69" s="5" t="n"/>
       <c r="I69" t="inlineStr">
         <is>
           <t>1:01:52.700000</t>
         </is>
       </c>
-      <c r="J69" t="n">
+      <c r="J69" s="5" t="n">
         <v>78.5</v>
       </c>
     </row>
@@ -5406,12 +5502,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H70" s="5" t="n"/>
       <c r="I70" t="inlineStr">
         <is>
           <t>1:01:56.720000</t>
         </is>
       </c>
-      <c r="J70" t="n">
+      <c r="J70" s="5" t="n">
         <v>78.40000000000001</v>
       </c>
     </row>
@@ -5440,12 +5537,13 @@
           <t>SPORTí</t>
         </is>
       </c>
+      <c r="H71" s="5" t="n"/>
       <c r="I71" t="inlineStr">
         <is>
           <t>1:02:24.460000</t>
         </is>
       </c>
-      <c r="J71" t="n">
+      <c r="J71" s="5" t="n">
         <v>77.8</v>
       </c>
     </row>
@@ -5474,12 +5572,13 @@
           <t>SIN CLUB</t>
         </is>
       </c>
+      <c r="H72" s="5" t="n"/>
       <c r="I72" t="inlineStr">
         <is>
           <t>1:02:42.640000</t>
         </is>
       </c>
-      <c r="J72" t="n">
+      <c r="J72" s="5" t="n">
         <v>77.40000000000001</v>
       </c>
     </row>
@@ -5508,12 +5607,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H73" s="5" t="n"/>
       <c r="I73" t="inlineStr">
         <is>
           <t>1:02:48.720000</t>
         </is>
       </c>
-      <c r="J73" t="n">
+      <c r="J73" s="5" t="n">
         <v>77.3</v>
       </c>
     </row>
@@ -5542,12 +5642,13 @@
           <t>PERCUTEAM</t>
         </is>
       </c>
+      <c r="H74" s="5" t="n"/>
       <c r="I74" t="inlineStr">
         <is>
           <t>1:02:51.700000</t>
         </is>
       </c>
-      <c r="J74" t="n">
+      <c r="J74" s="5" t="n">
         <v>77.2</v>
       </c>
     </row>
@@ -5576,12 +5677,13 @@
           <t>OCR ARAGON</t>
         </is>
       </c>
+      <c r="H75" s="5" t="n"/>
       <c r="I75" t="inlineStr">
         <is>
           <t>1:02:55.130000</t>
         </is>
       </c>
-      <c r="J75" t="n">
+      <c r="J75" s="5" t="n">
         <v>77.2</v>
       </c>
     </row>
@@ -5610,12 +5712,13 @@
           <t>Mallorca OCR</t>
         </is>
       </c>
+      <c r="H76" s="5" t="n"/>
       <c r="I76" t="inlineStr">
         <is>
           <t>1:03:44.680000</t>
         </is>
       </c>
-      <c r="J76" t="n">
+      <c r="J76" s="5" t="n">
         <v>76.2</v>
       </c>
     </row>
@@ -5644,12 +5747,13 @@
           <t>BRAVE BULLS</t>
         </is>
       </c>
+      <c r="H77" s="5" t="n"/>
       <c r="I77" t="inlineStr">
         <is>
           <t>1:03:46.060000</t>
         </is>
       </c>
-      <c r="J77" t="n">
+      <c r="J77" s="5" t="n">
         <v>76.09999999999999</v>
       </c>
     </row>
@@ -5678,12 +5782,13 @@
           <t>QUALIS</t>
         </is>
       </c>
+      <c r="H78" s="5" t="n"/>
       <c r="I78" t="inlineStr">
         <is>
           <t>1:04:27.920000</t>
         </is>
       </c>
-      <c r="J78" t="n">
+      <c r="J78" s="5" t="n">
         <v>75.3</v>
       </c>
     </row>
@@ -5712,12 +5817,13 @@
           <t>EstudioFit</t>
         </is>
       </c>
+      <c r="H79" s="5" t="n"/>
       <c r="I79" t="inlineStr">
         <is>
           <t>1:04:30.180000</t>
         </is>
       </c>
-      <c r="J79" t="n">
+      <c r="J79" s="5" t="n">
         <v>75.3</v>
       </c>
     </row>
@@ -5746,12 +5852,13 @@
           <t>RACERS LEGION MURCIA</t>
         </is>
       </c>
+      <c r="H80" s="5" t="n"/>
       <c r="I80" t="inlineStr">
         <is>
           <t>1:05:32.940000</t>
         </is>
       </c>
-      <c r="J80" t="n">
+      <c r="J80" s="5" t="n">
         <v>74.09999999999999</v>
       </c>
     </row>
@@ -5780,12 +5887,13 @@
           <t>THUNDER RACERS</t>
         </is>
       </c>
+      <c r="H81" s="5" t="n"/>
       <c r="I81" t="inlineStr">
         <is>
           <t>1:05:40.160000</t>
         </is>
       </c>
-      <c r="J81" t="n">
+      <c r="J81" s="5" t="n">
         <v>73.90000000000001</v>
       </c>
     </row>
@@ -5814,12 +5922,13 @@
           <t>TURIA RACERS</t>
         </is>
       </c>
+      <c r="H82" s="5" t="n"/>
       <c r="I82" t="inlineStr">
         <is>
           <t>1:05:47.910000</t>
         </is>
       </c>
-      <c r="J82" t="n">
+      <c r="J82" s="5" t="n">
         <v>73.8</v>
       </c>
     </row>
@@ -5848,12 +5957,13 @@
           <t>VB SPORT</t>
         </is>
       </c>
+      <c r="H83" s="5" t="n"/>
       <c r="I83" t="inlineStr">
         <is>
           <t>1:05:56.420000</t>
         </is>
       </c>
-      <c r="J83" t="n">
+      <c r="J83" s="5" t="n">
         <v>73.59999999999999</v>
       </c>
     </row>
@@ -5882,12 +5992,13 @@
           <t>OCR ARABA</t>
         </is>
       </c>
+      <c r="H84" s="5" t="n"/>
       <c r="I84" t="inlineStr">
         <is>
           <t>1:06:15.180000</t>
         </is>
       </c>
-      <c r="J84" t="n">
+      <c r="J84" s="5" t="n">
         <v>73.3</v>
       </c>
     </row>
@@ -5916,12 +6027,13 @@
           <t>MEDIEVALOCRTEAM</t>
         </is>
       </c>
+      <c r="H85" s="5" t="n"/>
       <c r="I85" t="inlineStr">
         <is>
           <t>1:06:22.890000</t>
         </is>
       </c>
-      <c r="J85" t="n">
+      <c r="J85" s="5" t="n">
         <v>73.09999999999999</v>
       </c>
     </row>
@@ -5950,12 +6062,13 @@
           <t>RACERS LEGION MURCIA</t>
         </is>
       </c>
+      <c r="H86" s="5" t="n"/>
       <c r="I86" t="inlineStr">
         <is>
           <t>1:07:04.330000</t>
         </is>
       </c>
-      <c r="J86" t="n">
+      <c r="J86" s="5" t="n">
         <v>72.40000000000001</v>
       </c>
     </row>
@@ -5979,12 +6092,13 @@
           <t>RACHITA Marian</t>
         </is>
       </c>
+      <c r="H87" s="5" t="n"/>
       <c r="I87" t="inlineStr">
         <is>
           <t>1:07:34.640000</t>
         </is>
       </c>
-      <c r="J87" t="n">
+      <c r="J87" s="5" t="n">
         <v>71.90000000000001</v>
       </c>
     </row>
@@ -6013,12 +6127,13 @@
           <t>PERCUTEAM</t>
         </is>
       </c>
+      <c r="H88" s="5" t="n"/>
       <c r="I88" t="inlineStr">
         <is>
           <t>1:07:39.390000</t>
         </is>
       </c>
-      <c r="J88" t="n">
+      <c r="J88" s="5" t="n">
         <v>71.8</v>
       </c>
     </row>
@@ -6047,12 +6162,13 @@
           <t>Lion Ocr</t>
         </is>
       </c>
+      <c r="H89" s="5" t="n"/>
       <c r="I89" t="inlineStr">
         <is>
           <t>1:07:42.930000</t>
         </is>
       </c>
-      <c r="J89" t="n">
+      <c r="J89" s="5" t="n">
         <v>71.7</v>
       </c>
     </row>
@@ -6081,12 +6197,13 @@
           <t>Mallorca OCR</t>
         </is>
       </c>
+      <c r="H90" s="5" t="n"/>
       <c r="I90" t="inlineStr">
         <is>
           <t>1:07:49.140000</t>
         </is>
       </c>
-      <c r="J90" t="n">
+      <c r="J90" s="5" t="n">
         <v>71.59999999999999</v>
       </c>
     </row>
@@ -6115,12 +6232,13 @@
           <t>RACERS LEGION ALICANTE</t>
         </is>
       </c>
+      <c r="H91" s="5" t="n"/>
       <c r="I91" t="inlineStr">
         <is>
           <t>1:08:02.890000</t>
         </is>
       </c>
-      <c r="J91" t="n">
+      <c r="J91" s="5" t="n">
         <v>71.40000000000001</v>
       </c>
     </row>
@@ -6149,12 +6267,13 @@
           <t>FOT-LI FIT</t>
         </is>
       </c>
+      <c r="H92" s="5" t="n"/>
       <c r="I92" t="inlineStr">
         <is>
           <t>1:08:09.890000</t>
         </is>
       </c>
-      <c r="J92" t="n">
+      <c r="J92" s="5" t="n">
         <v>71.2</v>
       </c>
     </row>
@@ -6183,12 +6302,13 @@
           <t>LA GATERA</t>
         </is>
       </c>
+      <c r="H93" s="5" t="n"/>
       <c r="I93" t="inlineStr">
         <is>
           <t>1:08:17.630000</t>
         </is>
       </c>
-      <c r="J93" t="n">
+      <c r="J93" s="5" t="n">
         <v>71.09999999999999</v>
       </c>
     </row>
@@ -6217,12 +6337,13 @@
           <t>TEAM RUINA</t>
         </is>
       </c>
+      <c r="H94" s="5" t="n"/>
       <c r="I94" t="inlineStr">
         <is>
           <t>1:08:19.330000</t>
         </is>
       </c>
-      <c r="J94" t="n">
+      <c r="J94" s="5" t="n">
         <v>71.09999999999999</v>
       </c>
     </row>
@@ -6251,12 +6372,13 @@
           <t>TEAM RUINA</t>
         </is>
       </c>
+      <c r="H95" s="5" t="n"/>
       <c r="I95" t="inlineStr">
         <is>
           <t>1:08:33.570000</t>
         </is>
       </c>
-      <c r="J95" t="n">
+      <c r="J95" s="5" t="n">
         <v>70.8</v>
       </c>
     </row>
@@ -6285,12 +6407,13 @@
           <t>T-RACE</t>
         </is>
       </c>
+      <c r="H96" s="5" t="n"/>
       <c r="I96" t="inlineStr">
         <is>
           <t>1:08:42.140000</t>
         </is>
       </c>
-      <c r="J96" t="n">
+      <c r="J96" s="5" t="n">
         <v>70.7</v>
       </c>
     </row>
@@ -6319,12 +6442,13 @@
           <t>AG CHILDRENS</t>
         </is>
       </c>
+      <c r="H97" s="5" t="n"/>
       <c r="I97" t="inlineStr">
         <is>
           <t>1:09:16.900000</t>
         </is>
       </c>
-      <c r="J97" t="n">
+      <c r="J97" s="5" t="n">
         <v>70.09999999999999</v>
       </c>
     </row>
@@ -6353,12 +6477,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H98" s="5" t="n"/>
       <c r="I98" t="inlineStr">
         <is>
           <t>1:09:19.060000</t>
         </is>
       </c>
-      <c r="J98" t="n">
+      <c r="J98" s="5" t="n">
         <v>70</v>
       </c>
     </row>
@@ -6387,12 +6512,13 @@
           <t>Brave Bulls Powered by Clonapure</t>
         </is>
       </c>
+      <c r="H99" s="5" t="n"/>
       <c r="I99" t="inlineStr">
         <is>
           <t>1:09:25.060000</t>
         </is>
       </c>
-      <c r="J99" t="n">
+      <c r="J99" s="5" t="n">
         <v>69.90000000000001</v>
       </c>
     </row>
@@ -6421,12 +6547,13 @@
           <t>PETRER - OCR ATHLETE</t>
         </is>
       </c>
+      <c r="H100" s="5" t="n"/>
       <c r="I100" t="inlineStr">
         <is>
           <t>1:09:25.200000</t>
         </is>
       </c>
-      <c r="J100" t="n">
+      <c r="J100" s="5" t="n">
         <v>69.90000000000001</v>
       </c>
     </row>
@@ -6455,12 +6582,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H101" s="5" t="n"/>
       <c r="I101" t="inlineStr">
         <is>
           <t>1:09:34.550000</t>
         </is>
       </c>
-      <c r="J101" t="n">
+      <c r="J101" s="5" t="n">
         <v>69.8</v>
       </c>
     </row>
@@ -6489,12 +6617,13 @@
           <t>FOT-LIFIT</t>
         </is>
       </c>
+      <c r="H102" s="5" t="n"/>
       <c r="I102" t="inlineStr">
         <is>
           <t>1:09:36.050000</t>
         </is>
       </c>
-      <c r="J102" t="n">
+      <c r="J102" s="5" t="n">
         <v>69.8</v>
       </c>
     </row>
@@ -6523,12 +6652,13 @@
           <t>MIKES GYM BY UNBROKEN TEAM</t>
         </is>
       </c>
+      <c r="H103" s="5" t="n"/>
       <c r="I103" t="inlineStr">
         <is>
           <t>1:10:09.610000</t>
         </is>
       </c>
-      <c r="J103" t="n">
+      <c r="J103" s="5" t="n">
         <v>69.2</v>
       </c>
     </row>
@@ -6557,12 +6687,13 @@
           <t>NGUP</t>
         </is>
       </c>
+      <c r="H104" s="5" t="n"/>
       <c r="I104" t="inlineStr">
         <is>
           <t>1:10:36.890000</t>
         </is>
       </c>
-      <c r="J104" t="n">
+      <c r="J104" s="5" t="n">
         <v>68.8</v>
       </c>
     </row>
@@ -6591,12 +6722,13 @@
           <t>ULTIMATE OCR</t>
         </is>
       </c>
+      <c r="H105" s="5" t="n"/>
       <c r="I105" t="inlineStr">
         <is>
           <t>1:10:48.080000</t>
         </is>
       </c>
-      <c r="J105" t="n">
+      <c r="J105" s="5" t="n">
         <v>68.59999999999999</v>
       </c>
     </row>
@@ -6625,12 +6757,13 @@
           <t>ZUAS SAB</t>
         </is>
       </c>
+      <c r="H106" s="5" t="n"/>
       <c r="I106" t="inlineStr">
         <is>
           <t>1:10:53.610000</t>
         </is>
       </c>
-      <c r="J106" t="n">
+      <c r="J106" s="5" t="n">
         <v>68.5</v>
       </c>
     </row>
@@ -6659,12 +6792,13 @@
           <t>QUALIS</t>
         </is>
       </c>
+      <c r="H107" s="5" t="n"/>
       <c r="I107" t="inlineStr">
         <is>
           <t>1:11:59.590000</t>
         </is>
       </c>
-      <c r="J107" t="n">
+      <c r="J107" s="5" t="n">
         <v>67.40000000000001</v>
       </c>
     </row>
@@ -6693,12 +6827,13 @@
           <t>SONS OF WORKOUT</t>
         </is>
       </c>
+      <c r="H108" s="5" t="n"/>
       <c r="I108" t="inlineStr">
         <is>
           <t>1:13:21.080000</t>
         </is>
       </c>
-      <c r="J108" t="n">
+      <c r="J108" s="5" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -6727,12 +6862,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H109" s="5" t="n"/>
       <c r="I109" t="inlineStr">
         <is>
           <t>1:13:50.330000</t>
         </is>
       </c>
-      <c r="J109" t="n">
+      <c r="J109" s="5" t="n">
         <v>65.8</v>
       </c>
     </row>
@@ -6761,12 +6897,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H110" s="5" t="n"/>
       <c r="I110" t="inlineStr">
         <is>
           <t>1:14:16.610000</t>
         </is>
       </c>
-      <c r="J110" t="n">
+      <c r="J110" s="5" t="n">
         <v>65.40000000000001</v>
       </c>
     </row>
@@ -6795,12 +6932,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H111" s="5" t="n"/>
       <c r="I111" t="inlineStr">
         <is>
           <t>1:15:26.560000</t>
         </is>
       </c>
-      <c r="J111" t="n">
+      <c r="J111" s="5" t="n">
         <v>64.40000000000001</v>
       </c>
     </row>
@@ -6829,12 +6967,13 @@
           <t>BRAVE BULLS</t>
         </is>
       </c>
+      <c r="H112" s="5" t="n"/>
       <c r="I112" t="inlineStr">
         <is>
           <t>1:15:57.300000</t>
         </is>
       </c>
-      <c r="J112" t="n">
+      <c r="J112" s="5" t="n">
         <v>63.9</v>
       </c>
     </row>
@@ -6863,12 +7002,13 @@
           <t>MIKES GYM</t>
         </is>
       </c>
+      <c r="H113" s="5" t="n"/>
       <c r="I113" t="inlineStr">
         <is>
           <t>1:16:26.740000</t>
         </is>
       </c>
-      <c r="J113" t="n">
+      <c r="J113" s="5" t="n">
         <v>63.5</v>
       </c>
     </row>
@@ -6897,12 +7037,13 @@
           <t>ROMPE LÍMITES OCR TEAM</t>
         </is>
       </c>
+      <c r="H114" s="5" t="n"/>
       <c r="I114" t="inlineStr">
         <is>
           <t>1:17:30.010000</t>
         </is>
       </c>
-      <c r="J114" t="n">
+      <c r="J114" s="5" t="n">
         <v>62.7</v>
       </c>
     </row>
@@ -6931,12 +7072,13 @@
           <t>THUNDER RACERS</t>
         </is>
       </c>
+      <c r="H115" s="5" t="n"/>
       <c r="I115" t="inlineStr">
         <is>
           <t>1:17:44.220000</t>
         </is>
       </c>
-      <c r="J115" t="n">
+      <c r="J115" s="5" t="n">
         <v>62.5</v>
       </c>
     </row>
@@ -6965,12 +7107,13 @@
           <t>MALLORCA OCR C.D</t>
         </is>
       </c>
+      <c r="H116" s="5" t="n"/>
       <c r="I116" t="inlineStr">
         <is>
           <t>1:18:29.070000</t>
         </is>
       </c>
-      <c r="J116" t="n">
+      <c r="J116" s="5" t="n">
         <v>61.9</v>
       </c>
     </row>
@@ -6999,12 +7142,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H117" s="5" t="n"/>
       <c r="I117" t="inlineStr">
         <is>
           <t>1:19:31.700000</t>
         </is>
       </c>
-      <c r="J117" t="n">
+      <c r="J117" s="5" t="n">
         <v>61.1</v>
       </c>
     </row>
@@ -7033,12 +7177,13 @@
           <t>SPORTI</t>
         </is>
       </c>
+      <c r="H118" s="5" t="n"/>
       <c r="I118" t="inlineStr">
         <is>
           <t>1:24:26.650000</t>
         </is>
       </c>
-      <c r="J118" t="n">
+      <c r="J118" s="5" t="n">
         <v>57.5</v>
       </c>
     </row>
@@ -7067,12 +7212,13 @@
           <t>Brave Bulls Powered by Clonapure</t>
         </is>
       </c>
+      <c r="H119" s="5" t="n"/>
       <c r="I119" t="inlineStr">
         <is>
           <t>1:25:37.140000</t>
         </is>
       </c>
-      <c r="J119" t="n">
+      <c r="J119" s="5" t="n">
         <v>56.7</v>
       </c>
     </row>
@@ -7101,12 +7247,13 @@
           <t>RACERS LEGION ALICANTE</t>
         </is>
       </c>
+      <c r="H120" s="5" t="n"/>
       <c r="I120" t="inlineStr">
         <is>
           <t>1:29:18.920000</t>
         </is>
       </c>
-      <c r="J120" t="n">
+      <c r="J120" s="5" t="n">
         <v>54.4</v>
       </c>
     </row>
@@ -7135,12 +7282,13 @@
           <t>PERCUTEAM</t>
         </is>
       </c>
+      <c r="H121" s="5" t="n"/>
       <c r="I121" t="inlineStr">
         <is>
           <t>1:31:29.650000</t>
         </is>
       </c>
-      <c r="J121" t="n">
+      <c r="J121" s="5" t="n">
         <v>53.1</v>
       </c>
     </row>
@@ -7169,12 +7317,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H122" s="5" t="n"/>
       <c r="I122" t="inlineStr">
         <is>
           <t>1:32:11.220000</t>
         </is>
       </c>
-      <c r="J122" t="n">
+      <c r="J122" s="5" t="n">
         <v>52.7</v>
       </c>
     </row>
@@ -7203,12 +7352,13 @@
           <t>OLLLU RACERS</t>
         </is>
       </c>
+      <c r="H123" s="5" t="n"/>
       <c r="I123" t="inlineStr">
         <is>
           <t>1:33:11.930000</t>
         </is>
       </c>
-      <c r="J123" t="n">
+      <c r="J123" s="5" t="n">
         <v>52.1</v>
       </c>
     </row>
@@ -7237,12 +7387,13 @@
           <t>ENTEP BOX</t>
         </is>
       </c>
+      <c r="H124" s="5" t="n"/>
       <c r="I124" t="inlineStr">
         <is>
           <t>1:35:24.470000</t>
         </is>
       </c>
-      <c r="J124" t="n">
+      <c r="J124" s="5" t="n">
         <v>50.9</v>
       </c>
     </row>
@@ -7266,12 +7417,13 @@
           <t>GARCIA Toni</t>
         </is>
       </c>
+      <c r="H125" s="5" t="n"/>
       <c r="I125" t="inlineStr">
         <is>
           <t>10:26:00.980000</t>
         </is>
       </c>
-      <c r="J125" t="n">
+      <c r="J125" s="5" t="n">
         <v>7.8</v>
       </c>
     </row>
@@ -7300,12 +7452,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H126" s="5" t="n"/>
       <c r="I126" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J126" t="n">
+      <c r="J126" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7334,12 +7487,13 @@
           <t>DENONTZAT</t>
         </is>
       </c>
+      <c r="H127" s="5" t="n"/>
       <c r="I127" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J127" t="n">
+      <c r="J127" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7368,12 +7522,13 @@
           <t>THUNDER RACERS</t>
         </is>
       </c>
+      <c r="H128" s="5" t="n"/>
       <c r="I128" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J128" t="n">
+      <c r="J128" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7402,12 +7557,13 @@
           <t>PERCUTEAM</t>
         </is>
       </c>
+      <c r="H129" s="5" t="n"/>
       <c r="I129" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J129" t="n">
+      <c r="J129" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7436,12 +7592,13 @@
           <t>QUALIS</t>
         </is>
       </c>
+      <c r="H130" s="5" t="n"/>
       <c r="I130" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J130" t="n">
+      <c r="J130" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7470,12 +7627,13 @@
           <t>BRAVE BULLS</t>
         </is>
       </c>
+      <c r="H131" s="5" t="n"/>
       <c r="I131" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J131" t="n">
+      <c r="J131" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7504,12 +7662,13 @@
           <t>PERCUTEAM</t>
         </is>
       </c>
+      <c r="H132" s="5" t="n"/>
       <c r="I132" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J132" t="n">
+      <c r="J132" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7538,12 +7697,13 @@
           <t>DENONTZAT</t>
         </is>
       </c>
+      <c r="H133" s="5" t="n"/>
       <c r="I133" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J133" t="n">
+      <c r="J133" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7572,12 +7732,13 @@
           <t>PERCUTEAM</t>
         </is>
       </c>
+      <c r="H134" s="5" t="n"/>
       <c r="I134" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J134" t="n">
+      <c r="J134" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7606,12 +7767,13 @@
           <t>PERCUTEAM</t>
         </is>
       </c>
+      <c r="H135" s="5" t="n"/>
       <c r="I135" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J135" t="n">
+      <c r="J135" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7640,12 +7802,13 @@
           <t>PERCUTEAM</t>
         </is>
       </c>
+      <c r="H136" s="5" t="n"/>
       <c r="I136" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J136" t="n">
+      <c r="J136" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7674,12 +7837,13 @@
           <t>EstudioFit</t>
         </is>
       </c>
+      <c r="H137" s="5" t="n"/>
       <c r="I137" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J137" t="n">
+      <c r="J137" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7708,12 +7872,13 @@
           <t>SPORTí</t>
         </is>
       </c>
+      <c r="H138" s="5" t="n"/>
       <c r="I138" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J138" t="n">
+      <c r="J138" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7742,12 +7907,13 @@
           <t>MIKES GYM</t>
         </is>
       </c>
+      <c r="H139" s="5" t="n"/>
       <c r="I139" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J139" t="n">
+      <c r="J139" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7776,12 +7942,13 @@
           <t>ORIGINAL BOX</t>
         </is>
       </c>
+      <c r="H140" s="5" t="n"/>
       <c r="I140" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J140" t="n">
+      <c r="J140" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7810,12 +7977,13 @@
           <t>RACERS LEGION MURCIA</t>
         </is>
       </c>
+      <c r="H141" s="5" t="n"/>
       <c r="I141" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J141" t="n">
+      <c r="J141" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7844,12 +8012,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H142" s="5" t="n"/>
       <c r="I142" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J142" t="n">
+      <c r="J142" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7878,12 +8047,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H143" s="5" t="n"/>
       <c r="I143" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J143" t="n">
+      <c r="J143" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7912,12 +8082,13 @@
           <t>TEAM RUINA</t>
         </is>
       </c>
+      <c r="H144" s="5" t="n"/>
       <c r="I144" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J144" t="n">
+      <c r="J144" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7946,12 +8117,13 @@
           <t>TEAM RUINA</t>
         </is>
       </c>
+      <c r="H145" s="5" t="n"/>
       <c r="I145" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J145" t="n">
+      <c r="J145" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7980,12 +8152,13 @@
           <t>TURIA RACERS</t>
         </is>
       </c>
+      <c r="H146" s="5" t="n"/>
       <c r="I146" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J146" t="n">
+      <c r="J146" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8014,12 +8187,13 @@
           <t>MIKES GYM</t>
         </is>
       </c>
+      <c r="H147" s="5" t="n"/>
       <c r="I147" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J147" t="n">
+      <c r="J147" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8062,61 +8236,61 @@
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
+      <c r="H1" s="2" t="n"/>
       <c r="I1" s="1" t="inlineStr">
         <is>
           <t>1   Unbroken Torrevieja 2024</t>
         </is>
       </c>
-      <c r="J1" s="1" t="n"/>
+      <c r="J1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Posición</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Puntos</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Carreras</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>Dorsal</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>Club</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>Categoría</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr">
         <is>
           <t>Posición</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="I2" s="3" t="inlineStr">
         <is>
           <t>Tiempo</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>Puntos</t>
         </is>
@@ -8147,12 +8321,13 @@
           <t>Epic Race</t>
         </is>
       </c>
+      <c r="H3" s="5" t="n"/>
       <c r="I3" t="inlineStr">
         <is>
           <t>1:08:13.140000</t>
         </is>
       </c>
-      <c r="J3" t="n">
+      <c r="J3" s="5" t="n">
         <v>100</v>
       </c>
     </row>
@@ -8181,12 +8356,13 @@
           <t>Epic Race</t>
         </is>
       </c>
+      <c r="H4" s="5" t="n"/>
       <c r="I4" t="inlineStr">
         <is>
           <t>1:09:13</t>
         </is>
       </c>
-      <c r="J4" t="n">
+      <c r="J4" s="5" t="n">
         <v>98.59999999999999</v>
       </c>
     </row>
@@ -8210,12 +8386,13 @@
           <t>Obrador Viel Carmina</t>
         </is>
       </c>
+      <c r="H5" s="5" t="n"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>1:11:41.600000</t>
         </is>
       </c>
-      <c r="J5" t="n">
+      <c r="J5" s="5" t="n">
         <v>95.2</v>
       </c>
     </row>
@@ -8244,12 +8421,13 @@
           <t>BRAVE BULLS</t>
         </is>
       </c>
+      <c r="H6" s="5" t="n"/>
       <c r="I6" t="inlineStr">
         <is>
           <t>1:14:58.580000</t>
         </is>
       </c>
-      <c r="J6" t="n">
+      <c r="J6" s="5" t="n">
         <v>91</v>
       </c>
     </row>
@@ -8278,12 +8456,13 @@
           <t>TEAM XXX BLACK MAMBA</t>
         </is>
       </c>
+      <c r="H7" s="5" t="n"/>
       <c r="I7" t="inlineStr">
         <is>
           <t>1:16:00.810000</t>
         </is>
       </c>
-      <c r="J7" t="n">
+      <c r="J7" s="5" t="n">
         <v>89.7</v>
       </c>
     </row>
@@ -8312,12 +8491,13 @@
           <t>ZUAS SAB</t>
         </is>
       </c>
+      <c r="H8" s="5" t="n"/>
       <c r="I8" t="inlineStr">
         <is>
           <t>1:16:24.550000</t>
         </is>
       </c>
-      <c r="J8" t="n">
+      <c r="J8" s="5" t="n">
         <v>89.3</v>
       </c>
     </row>
@@ -8346,12 +8526,13 @@
           <t>THE LAST TRAINING BY UNBROKEN PROTEAM</t>
         </is>
       </c>
+      <c r="H9" s="5" t="n"/>
       <c r="I9" t="inlineStr">
         <is>
           <t>1:19:28.280000</t>
         </is>
       </c>
-      <c r="J9" t="n">
+      <c r="J9" s="5" t="n">
         <v>85.8</v>
       </c>
     </row>
@@ -8380,12 +8561,13 @@
           <t>EPIC RACE</t>
         </is>
       </c>
+      <c r="H10" s="5" t="n"/>
       <c r="I10" t="inlineStr">
         <is>
           <t>1:20:14.260000</t>
         </is>
       </c>
-      <c r="J10" t="n">
+      <c r="J10" s="5" t="n">
         <v>85</v>
       </c>
     </row>
@@ -8414,12 +8596,13 @@
           <t>COMANDO NORTE</t>
         </is>
       </c>
+      <c r="H11" s="5" t="n"/>
       <c r="I11" t="inlineStr">
         <is>
           <t>1:20:21.760000</t>
         </is>
       </c>
-      <c r="J11" t="n">
+      <c r="J11" s="5" t="n">
         <v>84.90000000000001</v>
       </c>
     </row>
@@ -8448,12 +8631,13 @@
           <t>T-KONGS OCR</t>
         </is>
       </c>
+      <c r="H12" s="5" t="n"/>
       <c r="I12" t="inlineStr">
         <is>
           <t>1:20:37.260000</t>
         </is>
       </c>
-      <c r="J12" t="n">
+      <c r="J12" s="5" t="n">
         <v>84.59999999999999</v>
       </c>
     </row>
@@ -8482,12 +8666,13 @@
           <t>DENONTZAT</t>
         </is>
       </c>
+      <c r="H13" s="5" t="n"/>
       <c r="I13" t="inlineStr">
         <is>
           <t>1:23:18.480000</t>
         </is>
       </c>
-      <c r="J13" t="n">
+      <c r="J13" s="5" t="n">
         <v>81.90000000000001</v>
       </c>
     </row>
@@ -8516,12 +8701,13 @@
           <t>ENTEPBOX</t>
         </is>
       </c>
+      <c r="H14" s="5" t="n"/>
       <c r="I14" t="inlineStr">
         <is>
           <t>1:24:41.270000</t>
         </is>
       </c>
-      <c r="J14" t="n">
+      <c r="J14" s="5" t="n">
         <v>80.59999999999999</v>
       </c>
     </row>
@@ -8550,12 +8736,13 @@
           <t>APRIETA Y DISPARA</t>
         </is>
       </c>
+      <c r="H15" s="5" t="n"/>
       <c r="I15" t="inlineStr">
         <is>
           <t>1:27:33.190000</t>
         </is>
       </c>
-      <c r="J15" t="n">
+      <c r="J15" s="5" t="n">
         <v>77.90000000000001</v>
       </c>
     </row>
@@ -8584,12 +8771,13 @@
           <t>Brave Bulls Powered by Clonapure</t>
         </is>
       </c>
+      <c r="H16" s="5" t="n"/>
       <c r="I16" t="inlineStr">
         <is>
           <t>1:30:26.980000</t>
         </is>
       </c>
-      <c r="J16" t="n">
+      <c r="J16" s="5" t="n">
         <v>75.40000000000001</v>
       </c>
     </row>
@@ -8618,12 +8806,13 @@
           <t>BARRAKONG</t>
         </is>
       </c>
+      <c r="H17" s="5" t="n"/>
       <c r="I17" t="inlineStr">
         <is>
           <t>1:31:41.650000</t>
         </is>
       </c>
-      <c r="J17" t="n">
+      <c r="J17" s="5" t="n">
         <v>74.40000000000001</v>
       </c>
     </row>
@@ -8652,12 +8841,13 @@
           <t>Barrakong</t>
         </is>
       </c>
+      <c r="H18" s="5" t="n"/>
       <c r="I18" t="inlineStr">
         <is>
           <t>1:33:07.380000</t>
         </is>
       </c>
-      <c r="J18" t="n">
+      <c r="J18" s="5" t="n">
         <v>73.3</v>
       </c>
     </row>
@@ -8686,12 +8876,13 @@
           <t>THE NEST BOX</t>
         </is>
       </c>
+      <c r="H19" s="5" t="n"/>
       <c r="I19" t="inlineStr">
         <is>
           <t>1:35:54.440000</t>
         </is>
       </c>
-      <c r="J19" t="n">
+      <c r="J19" s="5" t="n">
         <v>71.09999999999999</v>
       </c>
     </row>
@@ -8720,12 +8911,13 @@
           <t>OLLURACERS</t>
         </is>
       </c>
+      <c r="H20" s="5" t="n"/>
       <c r="I20" t="inlineStr">
         <is>
           <t>1:38:07.830000</t>
         </is>
       </c>
-      <c r="J20" t="n">
+      <c r="J20" s="5" t="n">
         <v>69.5</v>
       </c>
     </row>
@@ -8754,12 +8946,13 @@
           <t>SPORTí</t>
         </is>
       </c>
+      <c r="H21" s="5" t="n"/>
       <c r="I21" t="inlineStr">
         <is>
           <t>1:38:21.670000</t>
         </is>
       </c>
-      <c r="J21" t="n">
+      <c r="J21" s="5" t="n">
         <v>69.40000000000001</v>
       </c>
     </row>
@@ -8788,12 +8981,13 @@
           <t>KIKOTRAINING TEAM</t>
         </is>
       </c>
+      <c r="H22" s="5" t="n"/>
       <c r="I22" t="inlineStr">
         <is>
           <t>1:41:47.890000</t>
         </is>
       </c>
-      <c r="J22" t="n">
+      <c r="J22" s="5" t="n">
         <v>67</v>
       </c>
     </row>
@@ -8822,12 +9016,13 @@
           <t>EPIC RACE</t>
         </is>
       </c>
+      <c r="H23" s="5" t="n"/>
       <c r="I23" t="inlineStr">
         <is>
           <t>1:41:52.190000</t>
         </is>
       </c>
-      <c r="J23" t="n">
+      <c r="J23" s="5" t="n">
         <v>67</v>
       </c>
     </row>
@@ -8856,12 +9051,13 @@
           <t>OCR-EX</t>
         </is>
       </c>
+      <c r="H24" s="5" t="n"/>
       <c r="I24" t="inlineStr">
         <is>
           <t>1:42:59.350000</t>
         </is>
       </c>
-      <c r="J24" t="n">
+      <c r="J24" s="5" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -8890,12 +9086,13 @@
           <t>CONTRA EL DIPG</t>
         </is>
       </c>
+      <c r="H25" s="5" t="n"/>
       <c r="I25" t="inlineStr">
         <is>
           <t>1:43:22.370000</t>
         </is>
       </c>
-      <c r="J25" t="n">
+      <c r="J25" s="5" t="n">
         <v>66</v>
       </c>
     </row>
@@ -8924,12 +9121,13 @@
           <t>QUALIS</t>
         </is>
       </c>
+      <c r="H26" s="5" t="n"/>
       <c r="I26" t="inlineStr">
         <is>
           <t>1:43:28.270000</t>
         </is>
       </c>
-      <c r="J26" t="n">
+      <c r="J26" s="5" t="n">
         <v>65.90000000000001</v>
       </c>
     </row>
@@ -8953,12 +9151,13 @@
           <t>CASTILLO MUÑOZ DE LEON MONTSE</t>
         </is>
       </c>
+      <c r="H27" s="5" t="n"/>
       <c r="I27" t="inlineStr">
         <is>
           <t>1:44:49.510000</t>
         </is>
       </c>
-      <c r="J27" t="n">
+      <c r="J27" s="5" t="n">
         <v>65.09999999999999</v>
       </c>
     </row>
@@ -8987,12 +9186,13 @@
           <t>ZUAS SAB</t>
         </is>
       </c>
+      <c r="H28" s="5" t="n"/>
       <c r="I28" t="inlineStr">
         <is>
           <t>1:47:44.970000</t>
         </is>
       </c>
-      <c r="J28" t="n">
+      <c r="J28" s="5" t="n">
         <v>63.3</v>
       </c>
     </row>
@@ -9021,12 +9221,13 @@
           <t>MEDIEVAL OCR TEAM</t>
         </is>
       </c>
+      <c r="H29" s="5" t="n"/>
       <c r="I29" t="inlineStr">
         <is>
           <t>1:47:59.230000</t>
         </is>
       </c>
-      <c r="J29" t="n">
+      <c r="J29" s="5" t="n">
         <v>63.2</v>
       </c>
     </row>
@@ -9055,12 +9256,13 @@
           <t>RACERS LEGION MURCIA</t>
         </is>
       </c>
+      <c r="H30" s="5" t="n"/>
       <c r="I30" t="inlineStr">
         <is>
           <t>1:50:01.710000</t>
         </is>
       </c>
-      <c r="J30" t="n">
+      <c r="J30" s="5" t="n">
         <v>62</v>
       </c>
     </row>
@@ -9089,12 +9291,13 @@
           <t>RACERS LEGION MURCIA</t>
         </is>
       </c>
+      <c r="H31" s="5" t="n"/>
       <c r="I31" t="inlineStr">
         <is>
           <t>1:51:06.200000</t>
         </is>
       </c>
-      <c r="J31" t="n">
+      <c r="J31" s="5" t="n">
         <v>61.4</v>
       </c>
     </row>
@@ -9123,12 +9326,13 @@
           <t>KIKOTRAINING</t>
         </is>
       </c>
+      <c r="H32" s="5" t="n"/>
       <c r="I32" t="inlineStr">
         <is>
           <t>1:53:01.180000</t>
         </is>
       </c>
-      <c r="J32" t="n">
+      <c r="J32" s="5" t="n">
         <v>60.4</v>
       </c>
     </row>
@@ -9157,12 +9361,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H33" s="5" t="n"/>
       <c r="I33" t="inlineStr">
         <is>
           <t>1:57:15.390000</t>
         </is>
       </c>
-      <c r="J33" t="n">
+      <c r="J33" s="5" t="n">
         <v>58.2</v>
       </c>
     </row>
@@ -9191,12 +9396,13 @@
           <t>RACERS LEGION ALICANTE</t>
         </is>
       </c>
+      <c r="H34" s="5" t="n"/>
       <c r="I34" t="inlineStr">
         <is>
           <t>1:58:37.120000</t>
         </is>
       </c>
-      <c r="J34" t="n">
+      <c r="J34" s="5" t="n">
         <v>57.5</v>
       </c>
     </row>
@@ -9225,12 +9431,13 @@
           <t>OLYMPUS TEAM ANDORRA</t>
         </is>
       </c>
+      <c r="H35" s="5" t="n"/>
       <c r="I35" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J35" t="n">
+      <c r="J35" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9259,12 +9466,13 @@
           <t>Fearless OCR</t>
         </is>
       </c>
+      <c r="H36" s="5" t="n"/>
       <c r="I36" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J36" t="n">
+      <c r="J36" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9293,12 +9501,13 @@
           <t>ENTEPBOX</t>
         </is>
       </c>
+      <c r="H37" s="5" t="n"/>
       <c r="I37" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J37" t="n">
+      <c r="J37" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9327,12 +9536,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H38" s="5" t="n"/>
       <c r="I38" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J38" t="n">
+      <c r="J38" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9361,12 +9571,13 @@
           <t>BRAVE BULLS</t>
         </is>
       </c>
+      <c r="H39" s="5" t="n"/>
       <c r="I39" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J39" t="n">
+      <c r="J39" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9395,12 +9606,13 @@
           <t>TURIA RACERS</t>
         </is>
       </c>
+      <c r="H40" s="5" t="n"/>
       <c r="I40" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J40" t="n">
+      <c r="J40" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9429,12 +9641,13 @@
           <t>Qualis</t>
         </is>
       </c>
+      <c r="H41" s="5" t="n"/>
       <c r="I41" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J41" t="n">
+      <c r="J41" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9463,12 +9676,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H42" s="5" t="n"/>
       <c r="I42" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J42" t="n">
+      <c r="J42" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9497,12 +9711,13 @@
           <t>BRAVE BULLS POWERED BY CLONAPURE</t>
         </is>
       </c>
+      <c r="H43" s="5" t="n"/>
       <c r="I43" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J43" t="n">
+      <c r="J43" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9531,12 +9746,13 @@
           <t>WARRIORS_T.E.A.M</t>
         </is>
       </c>
+      <c r="H44" s="5" t="n"/>
       <c r="I44" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J44" t="n">
+      <c r="J44" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9565,12 +9781,13 @@
           <t>Epic Race</t>
         </is>
       </c>
+      <c r="H45" s="5" t="n"/>
       <c r="I45" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J45" t="n">
+      <c r="J45" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9599,12 +9816,13 @@
           <t>RACERS LEGION ALICANTE</t>
         </is>
       </c>
+      <c r="H46" s="5" t="n"/>
       <c r="I46" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J46" t="n">
+      <c r="J46" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9633,12 +9851,13 @@
           <t>INDEPENDIENTE</t>
         </is>
       </c>
+      <c r="H47" s="5" t="n"/>
       <c r="I47" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J47" t="n">
+      <c r="J47" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9667,12 +9886,13 @@
           <t>RACER LEGION MURCIA</t>
         </is>
       </c>
+      <c r="H48" s="5" t="n"/>
       <c r="I48" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J48" t="n">
+      <c r="J48" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9701,12 +9921,13 @@
           <t>GLADIATOR TEAM</t>
         </is>
       </c>
+      <c r="H49" s="5" t="n"/>
       <c r="I49" t="inlineStr">
         <is>
           <t>Descalificado</t>
         </is>
       </c>
-      <c r="J49" t="n">
+      <c r="J49" s="5" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>